<commit_message>
148. Sort List.py 归并排序
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277D039D-5946-4E22-A43D-488D64FBD7FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220CDDB-C6AD-452F-B81F-FD347416DE7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,6 +39,26 @@
   </si>
   <si>
     <t>排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75（快排）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>148（归并排序）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>147（链表排序）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,10 +388,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -391,21 +414,30 @@
       <c r="A2" s="1">
         <v>43539</v>
       </c>
-      <c r="B2">
-        <v>147</v>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>148</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>75</v>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
author: dxs comment: c++ recursive solution for problem 148
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,10 @@
   </si>
   <si>
     <t>349（桶排序???)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -408,7 +412,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -450,6 +454,9 @@
       </c>
       <c r="C3" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
author: dxs comment: simple merge sort
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,22 @@
   </si>
   <si>
     <t>349（桶排序???)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53(dp)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88 merge sort</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -409,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -503,6 +519,25 @@
       </c>
       <c r="B8">
         <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: very easy problem
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB604D9-04C4-9F46-BEBE-EC3BF52F6D13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16416"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>排序</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>75（快排）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,23 +99,31 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 recursion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -151,7 +154,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,19 +431,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D17" sqref="D17:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -454,79 +458,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -534,29 +535,40 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
       <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43544</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
         <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -567,14 +579,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
author: dxs comment: cpp solution for 8 queens
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,6 +106,14 @@
   </si>
   <si>
     <t>70 recursion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51. N-Queens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -569,6 +577,17 @@
       </c>
       <c r="E11" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43545</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: easy dp
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,6 +110,14 @@
   </si>
   <si>
     <t>51. N-Queens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55 dp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -440,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -588,6 +596,17 @@
       </c>
       <c r="E12" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43545</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: simple dp for problem 64
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F64895C-CD5A-49D8-94FA-29B345CF6793}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
     <sheet name="复习计划" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,13 +152,21 @@
   </si>
   <si>
     <t>帅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64 dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,20 +485,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -508,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
@@ -522,7 +529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -533,7 +540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -547,7 +554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -555,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
@@ -566,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -580,7 +587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -588,7 +595,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -602,7 +609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
@@ -619,7 +626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43544</v>
       </c>
@@ -633,7 +640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43545</v>
       </c>
@@ -647,15 +654,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43545</v>
+        <v>43546</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43547</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -666,20 +684,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -693,7 +711,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>IF(新题!A2="","",新题!A2+7)</f>
         <v>43546</v>
@@ -703,7 +721,7 @@
         <v>147（链表排序）</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(新题!A3="","",新题!A3+7)</f>
         <v/>
@@ -713,7 +731,7 @@
         <v>148（归并排序）</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(新题!A4="","",新题!A4+7)</f>
         <v/>
@@ -723,7 +741,7 @@
         <v>75（快排）</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(新题!A5="","",新题!A5+7)</f>
         <v/>
@@ -733,7 +751,7 @@
         <v>349（桶排序???)</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>IF(新题!A6="","",新题!A6+7)</f>
         <v>43548</v>
@@ -743,7 +761,7 @@
         <v>355（堆）</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(新题!A7="","",新题!A7+7)</f>
         <v/>
@@ -753,7 +771,7 @@
         <v>164（桶排序）</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>IF(新题!A8="","",新题!A8+7)</f>
         <v>43549</v>
@@ -763,7 +781,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(新题!A9="","",新题!A9+7)</f>
         <v/>
@@ -773,7 +791,7 @@
         <v>53(dp)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>IF(新题!A10="","",新题!A10+7)</f>
         <v>43550</v>
@@ -783,19 +801,19 @@
         <v>88 merge sort</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>新题!B11</f>
         <v>70 recursion</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>新题!B12</f>
         <v>51. N-Queens</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>新题!B13</f>
         <v>55 dp</v>

</xml_diff>

<commit_message>
author: dxs comment: preorder traversal of binary tree
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,6 +160,14 @@
   </si>
   <si>
     <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>144 tree</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -486,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -674,6 +682,17 @@
       </c>
       <c r="E14" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43548</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: problem135,145
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4012DC73-221F-FD4A-8D31-B28C30FCAB23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
     <sheet name="复习计划" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -173,23 +172,31 @@
   </si>
   <si>
     <t>135 candy</t>
+  </si>
+  <si>
+    <t>145 tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -220,7 +227,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,20 +504,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -527,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
@@ -541,7 +548,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -552,7 +559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -566,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -574,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
@@ -585,7 +592,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -599,7 +606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -607,7 +614,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -621,7 +628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
@@ -638,7 +645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43544</v>
       </c>
@@ -652,7 +659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43545</v>
       </c>
@@ -666,7 +673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43546</v>
       </c>
@@ -677,7 +684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43547</v>
       </c>
@@ -688,7 +695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43548</v>
       </c>
@@ -702,7 +709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43548</v>
       </c>
@@ -711,6 +718,20 @@
       </c>
       <c r="D16" t="s">
         <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43548</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -721,20 +742,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -748,7 +769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>IF(新题!A2="","",新题!A2+7)</f>
         <v>43546</v>
@@ -758,7 +779,7 @@
         <v>147（链表排序）</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(新题!A3="","",新题!A3+7)</f>
         <v/>
@@ -768,7 +789,7 @@
         <v>148（归并排序）</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(新题!A4="","",新题!A4+7)</f>
         <v/>
@@ -778,7 +799,7 @@
         <v>75（快排）</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(新题!A5="","",新题!A5+7)</f>
         <v/>
@@ -788,7 +809,7 @@
         <v>349（桶排序???)</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>IF(新题!A6="","",新题!A6+7)</f>
         <v>43548</v>
@@ -798,7 +819,7 @@
         <v>355（堆）</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(新题!A7="","",新题!A7+7)</f>
         <v/>
@@ -808,7 +829,7 @@
         <v>164（桶排序）</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>IF(新题!A8="","",新题!A8+7)</f>
         <v>43549</v>
@@ -818,7 +839,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(新题!A9="","",新题!A9+7)</f>
         <v/>
@@ -828,7 +849,7 @@
         <v>53(dp)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>IF(新题!A10="","",新题!A10+7)</f>
         <v>43550</v>
@@ -838,19 +859,19 @@
         <v>88 merge sort</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>新题!B11</f>
         <v>70 recursion</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>新题!B12</f>
         <v>51. N-Queens</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>新题!B13</f>
         <v>55 dp</v>

</xml_diff>

<commit_message>
author: dxs comment: bst problem
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4A66A4-9136-D942-A221-0179C950ACC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="1540" windowWidth="16180" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12624" yWindow="1536" windowWidth="16176" windowHeight="11736"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">复习计划!$C$1:$F$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">新题!$C$1:$F$17</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,18 +226,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -269,7 +268,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,21 +545,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -580,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
@@ -597,7 +596,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -611,7 +610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -628,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -639,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
@@ -653,7 +652,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -670,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -679,7 +678,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -696,7 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
@@ -716,7 +715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43544</v>
       </c>
@@ -733,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43545</v>
       </c>
@@ -750,7 +749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43546</v>
       </c>
@@ -767,7 +766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43547</v>
       </c>
@@ -781,7 +780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43548</v>
       </c>
@@ -801,7 +800,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43548</v>
       </c>
@@ -821,7 +820,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43548</v>
       </c>
@@ -838,9 +837,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43550</v>
+        <v>43549</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -851,10 +850,13 @@
       <c r="E18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43550</v>
+        <v>43549</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
@@ -865,9 +867,12 @@
       <c r="E19" t="s">
         <v>19</v>
       </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F17" xr:uid="{861C8EDE-3583-4FBE-A0F3-96E41B702B78}"/>
+  <autoFilter ref="C1:F17"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -875,21 +880,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -909,7 +914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>IF(新题!A2="","",新题!A2+7)</f>
         <v>43546</v>
@@ -923,7 +928,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(新题!A3="","",新题!A3+7)</f>
         <v/>
@@ -937,7 +942,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(新题!A4="","",新题!A4+7)</f>
         <v/>
@@ -951,7 +956,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(新题!A5="","",新题!A5+7)</f>
         <v/>
@@ -965,7 +970,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>IF(新题!A6="","",新题!A6+7)</f>
         <v>43548</v>
@@ -979,7 +984,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(新题!A7="","",新题!A7+7)</f>
         <v/>
@@ -993,7 +998,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>IF(新题!A8="","",新题!A8+7)</f>
         <v>43549</v>
@@ -1007,7 +1012,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(新题!A9="","",新题!A9+7)</f>
         <v/>
@@ -1021,7 +1026,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>IF(新题!A10="","",新题!A10+7)</f>
         <v>43550</v>
@@ -1035,7 +1040,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>IF(新题!A11="","",新题!A11+7)</f>
         <v>43551</v>
@@ -1049,7 +1054,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>IF(新题!A12="","",新题!A12+7)</f>
         <v>43552</v>
@@ -1063,7 +1068,7 @@
         <v>Recursive</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>IF(新题!A13="","",新题!A13+7)</f>
         <v>43553</v>
@@ -1077,7 +1082,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>IF(新题!A14="","",新题!A14+7)</f>
         <v>43554</v>
@@ -1091,7 +1096,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>IF(新题!A15="","",新题!A15+7)</f>
         <v>43555</v>
@@ -1105,7 +1110,7 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>IF(新题!A16="","",新题!A16+7)</f>
         <v>43555</v>
@@ -1119,7 +1124,7 @@
         <v>Greedy</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>IF(新题!A17="","",新题!A17+7)</f>
         <v>43555</v>
@@ -1133,22 +1138,22 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>IF(新题!A18="","",新题!A18+7)</f>
-        <v>43557</v>
+        <v>43556</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>IF(新题!A19="","",新题!A19+7)</f>
-        <v>43557</v>
+        <v>43556</v>
       </c>
       <c r="C19" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F19" xr:uid="{753968E4-D4FA-4393-8D77-65A72AB01F42}"/>
+  <autoFilter ref="C1:F19"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
author: dxs comment: bfs for problem 102
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,6 +221,14 @@
   </si>
   <si>
     <t>Tree</t>
+  </si>
+  <si>
+    <t>102 bfs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -546,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -869,6 +877,17 @@
       </c>
       <c r="F19" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43550</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: simple dp for problem 413
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595D2696-3D7E-433A-A948-EB78286B0001}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13905" yWindow="1530" windowWidth="16170" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13908" yWindow="1536" windowWidth="16176" windowHeight="11736"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">复习计划!$C$1:$F$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">新题!$C$1:$F$17</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,12 +232,20 @@
   </si>
   <si>
     <t>tree</t>
+  </si>
+  <si>
+    <t>413 dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,21 +564,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -591,7 +598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
@@ -608,7 +615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -622,7 +629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -639,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -650,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
@@ -664,7 +671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -681,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -690,7 +697,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -707,7 +714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
@@ -727,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43544</v>
       </c>
@@ -744,7 +751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43545</v>
       </c>
@@ -761,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43546</v>
       </c>
@@ -778,7 +785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43547</v>
       </c>
@@ -792,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43548</v>
       </c>
@@ -812,7 +819,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43548</v>
       </c>
@@ -832,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43548</v>
       </c>
@@ -849,7 +856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43549</v>
       </c>
@@ -869,7 +876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43549</v>
       </c>
@@ -889,7 +896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43550</v>
       </c>
@@ -906,7 +913,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43550</v>
       </c>
@@ -923,7 +930,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43550</v>
       </c>
@@ -940,8 +947,19 @@
         <v>19</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43551</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:F17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:F17"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -949,21 +967,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -983,7 +1001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>IF(新题!A2="","",新题!A2+7)</f>
         <v>43546</v>
@@ -997,7 +1015,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(新题!A3="","",新题!A3+7)</f>
         <v/>
@@ -1011,7 +1029,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(新题!A4="","",新题!A4+7)</f>
         <v/>
@@ -1025,7 +1043,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(新题!A5="","",新题!A5+7)</f>
         <v/>
@@ -1039,7 +1057,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>IF(新题!A6="","",新题!A6+7)</f>
         <v>43548</v>
@@ -1053,7 +1071,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(新题!A7="","",新题!A7+7)</f>
         <v/>
@@ -1067,7 +1085,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>IF(新题!A8="","",新题!A8+7)</f>
         <v>43549</v>
@@ -1081,7 +1099,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(新题!A9="","",新题!A9+7)</f>
         <v/>
@@ -1095,7 +1113,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>IF(新题!A10="","",新题!A10+7)</f>
         <v>43550</v>
@@ -1109,7 +1127,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>IF(新题!A11="","",新题!A11+7)</f>
         <v>43551</v>
@@ -1123,7 +1141,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>IF(新题!A12="","",新题!A12+7)</f>
         <v>43552</v>
@@ -1137,7 +1155,7 @@
         <v>Recursive</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>IF(新题!A13="","",新题!A13+7)</f>
         <v>43553</v>
@@ -1151,7 +1169,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>IF(新题!A14="","",新题!A14+7)</f>
         <v>43554</v>
@@ -1165,7 +1183,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>IF(新题!A15="","",新题!A15+7)</f>
         <v>43555</v>
@@ -1179,7 +1197,7 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>IF(新题!A16="","",新题!A16+7)</f>
         <v>43555</v>
@@ -1193,7 +1211,7 @@
         <v>Greedy</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>IF(新题!A17="","",新题!A17+7)</f>
         <v>43555</v>
@@ -1207,14 +1225,14 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>IF(新题!A18="","",新题!A18+7)</f>
         <v>43556</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>IF(新题!A19="","",新题!A19+7)</f>
         <v>43556</v>
@@ -1222,7 +1240,7 @@
       <c r="C19" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F19" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="C1:F19"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
author: dxs comment: simple dp for problem 881
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -235,6 +235,14 @@
   </si>
   <si>
     <t>413 dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>881 dp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -565,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -956,6 +964,17 @@
       </c>
       <c r="F23" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43552</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: dp for 647
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -242,11 +242,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>881 dp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>done</t>
+    <t>647 dp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -573,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -971,10 +975,21 @@
         <v>43552</v>
       </c>
       <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
         <v>54</v>
       </c>
-      <c r="F24" t="s">
-        <v>55</v>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43552</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: hard dp for problem 887
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,6 +251,14 @@
   </si>
   <si>
     <t>647 dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>887 dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -990,6 +998,17 @@
       </c>
       <c r="F25" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43553</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: problem 304
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -255,6 +255,10 @@
   </si>
   <si>
     <t>887 dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -585,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1009,6 +1013,17 @@
       </c>
       <c r="F26" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43554</v>
+      </c>
+      <c r="B27">
+        <v>304</v>
+      </c>
+      <c r="F27" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: binary search for problem 719
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF23DF-82F2-471F-BE7D-F39345785C7E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13905" yWindow="1530" windowWidth="16170" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13908" yWindow="1536" windowWidth="16176" windowHeight="11736"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">复习计划!$C$1:$F$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">新题!$C$1:$F$17</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -268,13 +267,17 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -593,21 +596,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -627,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
@@ -644,7 +647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -658,7 +661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -675,7 +678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -686,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
@@ -700,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -717,7 +720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -726,7 +729,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -743,7 +746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
@@ -763,7 +766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43544</v>
       </c>
@@ -780,7 +783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43545</v>
       </c>
@@ -797,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43546</v>
       </c>
@@ -814,7 +817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43547</v>
       </c>
@@ -828,7 +831,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43548</v>
       </c>
@@ -848,7 +851,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43548</v>
       </c>
@@ -868,7 +871,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43548</v>
       </c>
@@ -885,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43549</v>
       </c>
@@ -905,7 +908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43549</v>
       </c>
@@ -925,7 +928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43550</v>
       </c>
@@ -942,7 +945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43550</v>
       </c>
@@ -959,7 +962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43550</v>
       </c>
@@ -976,7 +979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43551</v>
       </c>
@@ -990,7 +993,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43552</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43552</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43553</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43554</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43555</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43555</v>
       </c>
@@ -1062,8 +1065,19 @@
         <v>60</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43555</v>
+      </c>
+      <c r="B30">
+        <v>719</v>
+      </c>
+      <c r="F30" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:F17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:F17"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1071,21 +1085,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1105,7 +1119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>IF(新题!A2="","",新题!A2+7)</f>
         <v>43546</v>
@@ -1119,7 +1133,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(新题!A3="","",新题!A3+7)</f>
         <v/>
@@ -1133,7 +1147,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(新题!A4="","",新题!A4+7)</f>
         <v/>
@@ -1147,7 +1161,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(新题!A5="","",新题!A5+7)</f>
         <v/>
@@ -1161,7 +1175,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>IF(新题!A6="","",新题!A6+7)</f>
         <v>43548</v>
@@ -1175,7 +1189,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(新题!A7="","",新题!A7+7)</f>
         <v/>
@@ -1189,7 +1203,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>IF(新题!A8="","",新题!A8+7)</f>
         <v>43549</v>
@@ -1203,7 +1217,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(新题!A9="","",新题!A9+7)</f>
         <v/>
@@ -1217,7 +1231,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>IF(新题!A10="","",新题!A10+7)</f>
         <v>43550</v>
@@ -1231,7 +1245,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>IF(新题!A11="","",新题!A11+7)</f>
         <v>43551</v>
@@ -1245,7 +1259,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>IF(新题!A12="","",新题!A12+7)</f>
         <v>43552</v>
@@ -1259,7 +1273,7 @@
         <v>Recursive</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>IF(新题!A13="","",新题!A13+7)</f>
         <v>43553</v>
@@ -1273,7 +1287,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>IF(新题!A14="","",新题!A14+7)</f>
         <v>43554</v>
@@ -1287,7 +1301,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>IF(新题!A15="","",新题!A15+7)</f>
         <v>43555</v>
@@ -1301,7 +1315,7 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>IF(新题!A16="","",新题!A16+7)</f>
         <v>43555</v>
@@ -1315,7 +1329,7 @@
         <v>Greedy</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>IF(新题!A17="","",新题!A17+7)</f>
         <v>43555</v>
@@ -1329,14 +1343,14 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>IF(新题!A18="","",新题!A18+7)</f>
         <v>43556</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>IF(新题!A19="","",新题!A19+7)</f>
         <v>43556</v>
@@ -1344,7 +1358,7 @@
       <c r="C19" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F19" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="C1:F19"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
author: dxs comment: priority stack for problem 84
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E07147D-0930-4DCD-8264-1C030673DC50}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13905" yWindow="1530" windowWidth="16170" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13908" yWindow="1536" windowWidth="16176" windowHeight="11736"/>
   </bookViews>
   <sheets>
     <sheet name="新题" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">复习计划!$C$1:$F$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">新题!$C$1:$F$17</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -276,13 +275,17 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,21 +604,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -635,7 +638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43539</v>
       </c>
@@ -652,7 +655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -666,7 +669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -683,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -694,7 +697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43541</v>
       </c>
@@ -708,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -725,7 +728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43542</v>
       </c>
@@ -734,7 +737,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -751,7 +754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43543</v>
       </c>
@@ -771,7 +774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43544</v>
       </c>
@@ -788,7 +791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43545</v>
       </c>
@@ -805,7 +808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43546</v>
       </c>
@@ -822,7 +825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43547</v>
       </c>
@@ -836,7 +839,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43548</v>
       </c>
@@ -856,7 +859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43548</v>
       </c>
@@ -876,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43548</v>
       </c>
@@ -893,7 +896,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43549</v>
       </c>
@@ -913,7 +916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43549</v>
       </c>
@@ -933,7 +936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43550</v>
       </c>
@@ -950,7 +953,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43550</v>
       </c>
@@ -967,7 +970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43550</v>
       </c>
@@ -984,7 +987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43551</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43552</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43552</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43553</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43554</v>
       </c>
@@ -1054,7 +1057,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43555</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43555</v>
       </c>
@@ -1075,10 +1078,13 @@
       <c r="D29" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43555</v>
+        <v>43556</v>
       </c>
       <c r="B30">
         <v>719</v>
@@ -1088,7 +1094,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:F17"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1096,21 +1102,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>IF(新题!A2="","",新题!A2+7)</f>
         <v>43546</v>
@@ -1144,7 +1150,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(新题!A3="","",新题!A3+7)</f>
         <v/>
@@ -1158,7 +1164,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(新题!A4="","",新题!A4+7)</f>
         <v/>
@@ -1172,7 +1178,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(新题!A5="","",新题!A5+7)</f>
         <v/>
@@ -1186,7 +1192,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>IF(新题!A6="","",新题!A6+7)</f>
         <v>43548</v>
@@ -1200,7 +1206,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(新题!A7="","",新题!A7+7)</f>
         <v/>
@@ -1214,7 +1220,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>IF(新题!A8="","",新题!A8+7)</f>
         <v>43549</v>
@@ -1228,7 +1234,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(新题!A9="","",新题!A9+7)</f>
         <v/>
@@ -1242,7 +1248,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>IF(新题!A10="","",新题!A10+7)</f>
         <v>43550</v>
@@ -1256,7 +1262,7 @@
         <v>Sort</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>IF(新题!A11="","",新题!A11+7)</f>
         <v>43551</v>
@@ -1270,7 +1276,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>IF(新题!A12="","",新题!A12+7)</f>
         <v>43552</v>
@@ -1284,7 +1290,7 @@
         <v>Recursive</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>IF(新题!A13="","",新题!A13+7)</f>
         <v>43553</v>
@@ -1298,7 +1304,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>IF(新题!A14="","",新题!A14+7)</f>
         <v>43554</v>
@@ -1312,7 +1318,7 @@
         <v>DP</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>IF(新题!A15="","",新题!A15+7)</f>
         <v>43555</v>
@@ -1326,7 +1332,7 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>IF(新题!A16="","",新题!A16+7)</f>
         <v>43555</v>
@@ -1340,7 +1346,7 @@
         <v>Greedy</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>IF(新题!A17="","",新题!A17+7)</f>
         <v>43555</v>
@@ -1354,14 +1360,14 @@
         <v>Tree</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>IF(新题!A18="","",新题!A18+7)</f>
         <v>43556</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>IF(新题!A19="","",新题!A19+7)</f>
         <v>43556</v>
@@ -1369,7 +1375,7 @@
       <c r="C19" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F19" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="C1:F19"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
author: dxs comment: 552
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,6 +275,10 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -605,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1091,6 +1095,17 @@
       </c>
       <c r="F30" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43559</v>
+      </c>
+      <c r="B31">
+        <v>552</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: problem 837. edifying one.
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,6 +275,10 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -609,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1106,6 +1110,17 @@
       </c>
       <c r="F31" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43565</v>
+      </c>
+      <c r="B32">
+        <v>837</v>
+      </c>
+      <c r="F32" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: dp
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,6 +287,14 @@
   </si>
   <si>
     <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63 dp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1121,6 +1129,17 @@
       </c>
       <c r="F32" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43566</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: upload
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,7 +294,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>63 dp</t>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bfs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数论</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -621,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1111,35 +1127,108 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43559</v>
+        <v>43557</v>
       </c>
       <c r="B31">
-        <v>552</v>
+        <v>799</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43565</v>
+        <v>43558</v>
       </c>
       <c r="B32">
-        <v>837</v>
+        <v>845</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
+        <v>43559</v>
+      </c>
+      <c r="B33">
+        <v>552</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43560</v>
+      </c>
+      <c r="B34">
+        <v>542</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43561</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43563</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43564</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43565</v>
+      </c>
+      <c r="B39">
+        <v>837</v>
+      </c>
+      <c r="F39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>43566</v>
       </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="B40">
+        <v>63</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43567</v>
+      </c>
+      <c r="B41">
+        <v>372</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: none
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -641,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1262,6 +1262,20 @@
         <v>70</v>
       </c>
       <c r="F44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43576</v>
+      </c>
+      <c r="B45">
+        <v>376</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
author: dxs comment: simple question
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -311,6 +311,10 @@
   </si>
   <si>
     <t>数论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -641,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1277,6 +1281,17 @@
       </c>
       <c r="F45" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B46">
+        <v>228</v>
+      </c>
+      <c r="F46" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: a meaningful question
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -311,6 +311,10 @@
   </si>
   <si>
     <t>数论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -645,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1292,6 +1296,17 @@
       </c>
       <c r="F46" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43580</v>
+      </c>
+      <c r="B47">
+        <v>546</v>
+      </c>
+      <c r="F47" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: simple dp
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -649,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1307,6 +1307,17 @@
       </c>
       <c r="F47" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43582</v>
+      </c>
+      <c r="B48">
+        <v>935</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: no
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -311,6 +311,10 @@
   </si>
   <si>
     <t>数论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -649,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1318,6 +1322,17 @@
       </c>
       <c r="F48" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43585</v>
+      </c>
+      <c r="B49">
+        <v>848</v>
+      </c>
+      <c r="F49" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
author: dxs comment: good question
</commit_message>
<xml_diff>
--- a/Schedule/每日做题计划.xlsx
+++ b/Schedule/每日做题计划.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -311,6 +311,10 @@
   </si>
   <si>
     <t>数论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -653,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1333,6 +1337,17 @@
       </c>
       <c r="F49" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>